<commit_message>
Obtaining section allocations on the full updated solution
- changing the "-1" to -modVerNum for the new requests and full solution files
- modified the full solution file to include the lab name, section name, and section timeslot attributes - SectionAllocations.py uses this
- Also finalised 2021-Sem2-CAES-Wvl problem instance's Courses input file
</commit_message>
<xml_diff>
--- a/ifs-solver/src/main/resources/input/2021-Sem2-CAES-Wvl/Courses.xlsx
+++ b/ifs-solver/src/main/resources/input/2021-Sem2-CAES-Wvl/Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha\Documents\CS Honours\COMP700 - HP\student-lab-sectioning\ifs-solver\src\main\resources\input\2021-Sem2-CAES-Wvl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19734815-DCBB-4670-A03B-EA80B2D8A26B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CFB71C-AC2A-4B04-B46E-14D57EDB3FF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="58">
   <si>
     <t>course</t>
   </si>
@@ -88,12 +88,6 @@
   </si>
   <si>
     <t>BIOC202</t>
-  </si>
-  <si>
-    <t>BIOC308</t>
-  </si>
-  <si>
-    <t>BIOC316</t>
   </si>
   <si>
     <t>BIOL102</t>
@@ -532,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85:F85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,10 +737,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F10" s="1">
         <v>0.125</v>
@@ -757,33 +751,33 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E11" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F11" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1">
         <v>0.59027777777777779</v>
@@ -794,96 +788,96 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1">
-        <v>0.55208333333333337</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F13" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.47569444444444442</v>
       </c>
       <c r="F14" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="F15" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F16" s="1">
-        <v>0.125</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E17" s="1">
         <v>0.59027777777777779</v>
@@ -897,7 +891,7 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -906,27 +900,27 @@
         <v>9</v>
       </c>
       <c r="E18" s="1">
-        <v>0.47569444444444442</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F18" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1">
-        <v>0.55208333333333337</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="F19" s="1">
         <v>3.125E-2</v>
@@ -934,10 +928,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -949,12 +943,12 @@
         <v>0.39930555555555558</v>
       </c>
       <c r="F20" s="1">
-        <v>0.10416666666666667</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -963,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1">
         <v>0.59027777777777779</v>
@@ -977,39 +971,39 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E22" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.51388888888888895</v>
       </c>
       <c r="F22" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E23" s="1">
-        <v>0.3611111111111111</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F23" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1020,13 +1014,13 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F24" s="1">
         <v>0.125</v>
@@ -1034,19 +1028,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E25" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F25" s="1">
         <v>0.125</v>
@@ -1054,36 +1048,36 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E26" s="1">
-        <v>0.51388888888888895</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F26" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E27" s="1">
         <v>0.59027777777777779</v>
@@ -1094,16 +1088,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E28" s="1">
         <v>0.59027777777777779</v>
@@ -1114,73 +1108,73 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="F29" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E30" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="F30" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E31" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="F31" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -1197,19 +1191,19 @@
         <v>25</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E33" s="1">
-        <v>0.55208333333333337</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F33" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1217,19 +1211,19 @@
         <v>25</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1">
-        <v>0.55208333333333337</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F34" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1243,18 +1237,18 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E35" s="1">
-        <v>0.3611111111111111</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F35" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1263,18 +1257,21 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E36" s="1">
         <v>0.59027777777777779</v>
       </c>
       <c r="F36" s="1">
         <v>0.125</v>
+      </c>
+      <c r="G36">
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1283,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E37" s="1">
         <v>0.59027777777777779</v>
@@ -1294,16 +1291,16 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E38" s="1">
         <v>0.59027777777777779</v>
@@ -1326,7 +1323,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F39" s="1">
         <v>0.125</v>
@@ -1334,7 +1331,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1343,21 +1340,18 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E40" s="1">
         <v>0.59027777777777779</v>
       </c>
       <c r="F40" s="1">
         <v>0.125</v>
-      </c>
-      <c r="G40">
-        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1366,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E41" s="1">
         <v>0.59027777777777779</v>
@@ -1377,16 +1371,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E42" s="1">
         <v>0.59027777777777779</v>
@@ -1397,16 +1391,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E43" s="1">
         <v>0.59027777777777779</v>
@@ -1417,7 +1411,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1426,10 +1420,10 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E44" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F44" s="1">
         <v>0.125</v>
@@ -1437,16 +1431,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E45" s="1">
         <v>0.59027777777777779</v>
@@ -1457,16 +1451,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E46" s="1">
         <v>0.59027777777777779</v>
@@ -1477,13 +1471,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
@@ -1506,10 +1500,10 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E48" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F48" s="1">
         <v>0.125</v>
@@ -1526,7 +1520,7 @@
         <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E49" s="1">
         <v>0.59027777777777779</v>
@@ -1537,7 +1531,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -1546,7 +1540,7 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E50" s="1">
         <v>0.59027777777777779</v>
@@ -1557,16 +1551,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E51" s="1">
         <v>0.59027777777777779</v>
@@ -1577,7 +1571,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -1597,7 +1591,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1606,7 +1600,7 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E53" s="1">
         <v>0.59027777777777779</v>
@@ -1617,7 +1611,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -1637,7 +1631,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1646,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E55" s="1">
         <v>0.59027777777777779</v>
@@ -1663,13 +1657,13 @@
         <v>1</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E56" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F56" s="1">
         <v>0.125</v>
@@ -1677,16 +1671,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E57" s="1">
         <v>0.59027777777777779</v>
@@ -1697,7 +1691,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1706,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E58" s="1">
         <v>0.59027777777777779</v>
@@ -1717,7 +1711,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1726,10 +1720,10 @@
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E59" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F59" s="1">
         <v>0.125</v>
@@ -1737,19 +1731,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F60" s="1">
         <v>0.125</v>
@@ -1757,7 +1751,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -1766,10 +1760,10 @@
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E61" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F61" s="1">
         <v>0.125</v>
@@ -1777,22 +1771,22 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E62" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="F62" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1806,10 +1800,10 @@
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E63" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F63" s="1">
         <v>0.125</v>
@@ -1817,7 +1811,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1826,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E64" s="1">
         <v>0.59027777777777779</v>
@@ -1846,10 +1840,10 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E65" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F65" s="1">
         <v>0.125</v>
@@ -1860,33 +1854,33 @@
         <v>38</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D66" t="s">
         <v>6</v>
       </c>
       <c r="E66" s="1">
-        <v>0.55208333333333337</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F66" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E67" s="1">
         <v>0.59027777777777779</v>
@@ -1917,7 +1911,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -1937,13 +1931,13 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D70" t="s">
         <v>6</v>
@@ -1957,16 +1951,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E71" s="1">
         <v>0.59027777777777779</v>
@@ -1977,16 +1971,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B72">
         <v>1</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E72" s="1">
         <v>0.59027777777777779</v>
@@ -2000,44 +1994,44 @@
         <v>55</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E73" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.4375</v>
       </c>
       <c r="F73" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E74" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.55208333333333337</v>
       </c>
       <c r="F74" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2046,7 +2040,7 @@
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E75" s="1">
         <v>0.59027777777777779</v>
@@ -2057,7 +2051,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2066,10 +2060,10 @@
         <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E76" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F76" s="1">
         <v>0.125</v>
@@ -2077,47 +2071,47 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C77">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E77" s="1">
-        <v>0.4375</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F77" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E78" s="1">
-        <v>0.55208333333333337</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F78" s="1">
-        <v>3.125E-2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2126,10 +2120,10 @@
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E79" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F79" s="1">
         <v>0.125</v>
@@ -2137,13 +2131,13 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="B80">
         <v>1</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
@@ -2157,16 +2151,16 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
       <c r="C81">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E81" s="1">
         <v>0.59027777777777779</v>
@@ -2177,50 +2171,50 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E82" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="F82" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B83">
         <v>1</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E83" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.62847222222222221</v>
       </c>
       <c r="F83" s="1">
-        <v>0.125</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -2232,18 +2226,18 @@
         <v>0.39930555555555558</v>
       </c>
       <c r="F84" s="1">
-        <v>0.125</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D85" t="s">
         <v>9</v>
@@ -2252,86 +2246,6 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="F85" s="1">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>43</v>
-      </c>
-      <c r="B86">
-        <v>1</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86" t="s">
-        <v>5</v>
-      </c>
-      <c r="E86" s="1">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="F86" s="1">
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>43</v>
-      </c>
-      <c r="B87">
-        <v>1</v>
-      </c>
-      <c r="C87">
-        <v>2</v>
-      </c>
-      <c r="D87" t="s">
-        <v>8</v>
-      </c>
-      <c r="E87" s="1">
-        <v>0.62847222222222221</v>
-      </c>
-      <c r="F87" s="1">
-        <v>3.125E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>43</v>
-      </c>
-      <c r="B88">
-        <v>2</v>
-      </c>
-      <c r="C88">
-        <v>1</v>
-      </c>
-      <c r="D88" t="s">
-        <v>7</v>
-      </c>
-      <c r="E88" s="1">
-        <v>0.39930555555555558</v>
-      </c>
-      <c r="F88" s="1">
-        <v>6.25E-2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>43</v>
-      </c>
-      <c r="B89">
-        <v>2</v>
-      </c>
-      <c r="C89">
-        <v>2</v>
-      </c>
-      <c r="D89" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="1">
-        <v>0.59027777777777779</v>
-      </c>
-      <c r="F89" s="1">
         <v>6.25E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Experimentation: 2021-Sem2-CAES-Wvl: Initial solution
</commit_message>
<xml_diff>
--- a/ifs-solver/src/main/resources/input/2021-Sem2-CAES-Wvl/Courses.xlsx
+++ b/ifs-solver/src/main/resources/input/2021-Sem2-CAES-Wvl/Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha\Documents\CS Honours\COMP700 - HP\student-lab-sectioning\ifs-solver\src\main\resources\input\2021-Sem2-CAES-Wvl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CFB71C-AC2A-4B04-B46E-14D57EDB3FF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634379D0-B699-4F96-BF41-C69F840D6C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,6 +585,9 @@
       <c r="F2" s="1">
         <v>0.125</v>
       </c>
+      <c r="G2">
+        <v>500</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -605,6 +608,9 @@
       <c r="F3" s="1">
         <v>0.125</v>
       </c>
+      <c r="G3">
+        <v>500</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -625,6 +631,9 @@
       <c r="F4" s="1">
         <v>0.10416666666666667</v>
       </c>
+      <c r="G4">
+        <v>500</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -645,6 +654,9 @@
       <c r="F5" s="1">
         <v>3.125E-2</v>
       </c>
+      <c r="G5">
+        <v>500</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -665,6 +677,9 @@
       <c r="F6" s="1">
         <v>3.125E-2</v>
       </c>
+      <c r="G6">
+        <v>500</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -685,6 +700,9 @@
       <c r="F7" s="1">
         <v>0.10416666666666667</v>
       </c>
+      <c r="G7">
+        <v>500</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -705,6 +723,9 @@
       <c r="F8" s="1">
         <v>0.10416666666666667</v>
       </c>
+      <c r="G8">
+        <v>500</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -725,6 +746,9 @@
       <c r="F9" s="1">
         <v>3.125E-2</v>
       </c>
+      <c r="G9">
+        <v>500</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -745,6 +769,9 @@
       <c r="F10" s="1">
         <v>0.125</v>
       </c>
+      <c r="G10">
+        <v>500</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -765,6 +792,9 @@
       <c r="F11" s="1">
         <v>0.125</v>
       </c>
+      <c r="G11">
+        <v>500</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -785,6 +815,9 @@
       <c r="F12" s="1">
         <v>0.125</v>
       </c>
+      <c r="G12">
+        <v>500</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -805,6 +838,9 @@
       <c r="F13" s="1">
         <v>0.125</v>
       </c>
+      <c r="G13">
+        <v>500</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -825,6 +861,9 @@
       <c r="F14" s="1">
         <v>3.125E-2</v>
       </c>
+      <c r="G14">
+        <v>500</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -845,6 +884,9 @@
       <c r="F15" s="1">
         <v>3.125E-2</v>
       </c>
+      <c r="G15">
+        <v>500</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -865,8 +907,11 @@
       <c r="F16" s="1">
         <v>0.10416666666666667</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -885,8 +930,11 @@
       <c r="F17" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -905,8 +953,11 @@
       <c r="F18" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -925,8 +976,11 @@
       <c r="F19" s="1">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -945,8 +999,11 @@
       <c r="F20" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -965,8 +1022,11 @@
       <c r="F21" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -985,8 +1045,11 @@
       <c r="F22" s="1">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1005,8 +1068,11 @@
       <c r="F23" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1025,8 +1091,11 @@
       <c r="F24" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1045,8 +1114,11 @@
       <c r="F25" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1065,8 +1137,11 @@
       <c r="F26" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1085,8 +1160,11 @@
       <c r="F27" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1105,8 +1183,11 @@
       <c r="F28" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1125,8 +1206,11 @@
       <c r="F29" s="1">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1145,8 +1229,11 @@
       <c r="F30" s="1">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -1165,8 +1252,11 @@
       <c r="F31" s="1">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1184,6 +1274,9 @@
       </c>
       <c r="F32" s="1">
         <v>0.125</v>
+      </c>
+      <c r="G32">
+        <v>500</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1205,6 +1298,9 @@
       <c r="F33" s="1">
         <v>0.125</v>
       </c>
+      <c r="G33">
+        <v>500</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1225,6 +1321,9 @@
       <c r="F34" s="1">
         <v>0.125</v>
       </c>
+      <c r="G34">
+        <v>500</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -1245,6 +1344,9 @@
       <c r="F35" s="1">
         <v>0.125</v>
       </c>
+      <c r="G35">
+        <v>500</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1266,7 +1368,7 @@
         <v>0.125</v>
       </c>
       <c r="G36">
-        <v>200</v>
+        <v>500</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1288,6 +1390,9 @@
       <c r="F37" s="1">
         <v>0.125</v>
       </c>
+      <c r="G37">
+        <v>500</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1308,6 +1413,9 @@
       <c r="F38" s="1">
         <v>0.125</v>
       </c>
+      <c r="G38">
+        <v>500</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1328,6 +1436,9 @@
       <c r="F39" s="1">
         <v>0.125</v>
       </c>
+      <c r="G39">
+        <v>500</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1348,6 +1459,9 @@
       <c r="F40" s="1">
         <v>0.125</v>
       </c>
+      <c r="G40">
+        <v>500</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1368,6 +1482,9 @@
       <c r="F41" s="1">
         <v>0.125</v>
       </c>
+      <c r="G41">
+        <v>500</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1388,6 +1505,9 @@
       <c r="F42" s="1">
         <v>0.125</v>
       </c>
+      <c r="G42">
+        <v>500</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1408,6 +1528,9 @@
       <c r="F43" s="1">
         <v>0.125</v>
       </c>
+      <c r="G43">
+        <v>500</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1428,6 +1551,9 @@
       <c r="F44" s="1">
         <v>0.125</v>
       </c>
+      <c r="G44">
+        <v>500</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1448,6 +1574,9 @@
       <c r="F45" s="1">
         <v>0.125</v>
       </c>
+      <c r="G45">
+        <v>500</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -1468,6 +1597,9 @@
       <c r="F46" s="1">
         <v>0.125</v>
       </c>
+      <c r="G46">
+        <v>500</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1488,6 +1620,9 @@
       <c r="F47" s="1">
         <v>0.125</v>
       </c>
+      <c r="G47">
+        <v>500</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1508,8 +1643,11 @@
       <c r="F48" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1528,8 +1666,11 @@
       <c r="F49" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>30</v>
       </c>
@@ -1548,8 +1689,11 @@
       <c r="F50" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -1568,8 +1712,11 @@
       <c r="F51" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -1588,8 +1735,11 @@
       <c r="F52" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>32</v>
       </c>
@@ -1608,8 +1758,11 @@
       <c r="F53" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>33</v>
       </c>
@@ -1628,8 +1781,11 @@
       <c r="F54" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>34</v>
       </c>
@@ -1648,8 +1804,11 @@
       <c r="F55" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>34</v>
       </c>
@@ -1668,8 +1827,11 @@
       <c r="F56" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>35</v>
       </c>
@@ -1688,8 +1850,11 @@
       <c r="F57" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>49</v>
       </c>
@@ -1708,8 +1873,11 @@
       <c r="F58" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>50</v>
       </c>
@@ -1728,8 +1896,11 @@
       <c r="F59" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>51</v>
       </c>
@@ -1748,8 +1919,11 @@
       <c r="F60" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -1768,8 +1942,11 @@
       <c r="F61" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>36</v>
       </c>
@@ -1788,8 +1965,11 @@
       <c r="F62" s="1">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>52</v>
       </c>
@@ -1808,8 +1988,11 @@
       <c r="F63" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -1828,8 +2011,11 @@
       <c r="F64" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -1848,8 +2034,11 @@
       <c r="F65" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -1868,8 +2057,11 @@
       <c r="F66" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>38</v>
       </c>
@@ -1888,8 +2080,11 @@
       <c r="F67" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>39</v>
       </c>
@@ -1908,8 +2103,11 @@
       <c r="F68" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>53</v>
       </c>
@@ -1928,8 +2126,11 @@
       <c r="F69" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>54</v>
       </c>
@@ -1948,8 +2149,11 @@
       <c r="F70" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>55</v>
       </c>
@@ -1968,8 +2172,11 @@
       <c r="F71" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>55</v>
       </c>
@@ -1988,8 +2195,11 @@
       <c r="F72" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>55</v>
       </c>
@@ -2008,8 +2218,11 @@
       <c r="F73" s="1">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>55</v>
       </c>
@@ -2028,8 +2241,11 @@
       <c r="F74" s="1">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -2048,8 +2264,11 @@
       <c r="F75" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -2068,8 +2287,11 @@
       <c r="F76" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -2088,8 +2310,11 @@
       <c r="F77" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -2108,8 +2333,11 @@
       <c r="F78" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>40</v>
       </c>
@@ -2128,8 +2356,11 @@
       <c r="F79" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>56</v>
       </c>
@@ -2148,8 +2379,11 @@
       <c r="F80" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>57</v>
       </c>
@@ -2168,8 +2402,11 @@
       <c r="F81" s="1">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>41</v>
       </c>
@@ -2188,8 +2425,11 @@
       <c r="F82" s="1">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>41</v>
       </c>
@@ -2208,8 +2448,11 @@
       <c r="F83" s="1">
         <v>3.125E-2</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>41</v>
       </c>
@@ -2228,8 +2471,11 @@
       <c r="F84" s="1">
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>41</v>
       </c>
@@ -2247,6 +2493,9 @@
       </c>
       <c r="F85" s="1">
         <v>6.25E-2</v>
+      </c>
+      <c r="G85">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>